<commit_message>
Optimized and Median val. added
</commit_message>
<xml_diff>
--- a/Makes.xlsx
+++ b/Makes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,21 @@
           <t>Make</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Median Price</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Median Mileage</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Median Year</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,22 +496,31 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7488742-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7656942-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E2" t="n">
         <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>212542</v>
+        <v>208000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H2" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I2" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="3">
@@ -506,26 +530,35 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23800</v>
+        <v>23500</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7446216-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7656718-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E3" t="n">
         <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>158000</v>
+        <v>189000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H3" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I3" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="4">
@@ -535,11 +568,11 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19300</v>
+        <v>22300</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7600700-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7637801-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -549,12 +582,21 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>283683</v>
+        <v>279000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H4" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I4" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="5">
@@ -564,26 +606,35 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25000</v>
+        <v>20900</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7618076-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7578444-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>250000</v>
+        <v>126000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H5" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I5" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="6">
@@ -593,11 +644,11 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24800</v>
+        <v>22000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7420489-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7654556-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -607,12 +658,21 @@
         <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>225000</v>
+        <v>240000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H6" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I6" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="7">
@@ -622,26 +682,35 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>20900</v>
+        <v>22900</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7578444-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7655719-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>126000</v>
+        <v>274444</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H7" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I7" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="8">
@@ -651,26 +720,35 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>23200</v>
+        <v>22500</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7526678-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7654167-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>182814</v>
+        <v>378785</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H8" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I8" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="9">
@@ -680,26 +758,35 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>22500</v>
+        <v>25000</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7629165-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7618076-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>198000</v>
+        <v>250000</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H9" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I9" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="10">
@@ -709,26 +796,35 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>20500</v>
+        <v>20000</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7646008-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7624790-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>2007</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="F10" t="n">
-        <v>214000</v>
+        <v>206000</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H10" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I10" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="11">
@@ -738,11 +834,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>23500</v>
+        <v>23200</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7643678-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7526678-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -752,12 +848,21 @@
         <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>200000</v>
+        <v>182814</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H11" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I11" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="12">
@@ -767,11 +872,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23500</v>
+        <v>21500</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7603261-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7488742-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -781,12 +886,21 @@
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>171000</v>
+        <v>212542</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H12" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I12" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="13">
@@ -796,26 +910,35 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17600</v>
+        <v>24800</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7643271-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7420489-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>235000</v>
+        <v>225000</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H13" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I13" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="14">
@@ -825,26 +948,35 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>22700</v>
+        <v>17600</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7626518-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7643271-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E14" t="n">
         <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>224000</v>
+        <v>235000</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H14" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I14" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="15">
@@ -854,11 +986,11 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>24500</v>
+        <v>22800</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7618153-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7650430-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -868,12 +1000,21 @@
         <v>3</v>
       </c>
       <c r="F15" t="n">
-        <v>196000</v>
+        <v>186000</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H15" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I15" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="16">
@@ -883,26 +1024,35 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23900</v>
+        <v>22500</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7596570-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7629165-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E16" t="n">
         <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>225000</v>
+        <v>198000</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H16" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I16" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="17">
@@ -912,26 +1062,35 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>25000</v>
+        <v>23500</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7640715-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7643678-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E17" t="n">
         <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>173000</v>
+        <v>200000</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H17" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I17" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="18">
@@ -941,26 +1100,35 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>21300</v>
+        <v>23500</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7640289-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7603261-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E18" t="n">
         <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>165466</v>
+        <v>171000</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H18" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I18" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="19">
@@ -970,26 +1138,35 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>23000</v>
+        <v>22700</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7615919-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7626518-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E19" t="n">
         <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>255000</v>
+        <v>224000</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H19" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I19" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="20">
@@ -999,11 +1176,11 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>23000</v>
+        <v>24500</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7638414-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7618153-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1013,12 +1190,21 @@
         <v>3</v>
       </c>
       <c r="F20" t="n">
-        <v>260000</v>
+        <v>196000</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H20" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I20" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="21">
@@ -1028,26 +1214,35 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>22800</v>
+        <v>23900</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7637801-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7596570-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E21" t="n">
         <v>3</v>
       </c>
       <c r="F21" t="n">
-        <v>279000</v>
+        <v>225000</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H21" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I21" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="22">
@@ -1057,26 +1252,35 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>22300</v>
+        <v>25000</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7582833-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7640715-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E22" t="n">
         <v>3</v>
       </c>
       <c r="F22" t="n">
-        <v>270000</v>
+        <v>173000</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H22" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I22" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="23">
@@ -1086,11 +1290,11 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>22800</v>
+        <v>21300</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7634532-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7640289-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1100,12 +1304,21 @@
         <v>3</v>
       </c>
       <c r="F23" t="n">
-        <v>298000</v>
+        <v>165466</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H23" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I23" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="24">
@@ -1119,22 +1332,31 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7635502-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7615919-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E24" t="n">
         <v>3</v>
       </c>
       <c r="F24" t="n">
-        <v>260000</v>
+        <v>255000</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H24" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I24" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="25">
@@ -1144,11 +1366,11 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21000</v>
+        <v>23000</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7627049-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7638414-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1158,12 +1380,21 @@
         <v>3</v>
       </c>
       <c r="F25" t="n">
-        <v>163059</v>
+        <v>260000</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H25" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I25" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="26">
@@ -1173,11 +1404,11 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>22000</v>
+        <v>22300</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7634880-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7582833-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1187,12 +1418,21 @@
         <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>245368</v>
+        <v>270000</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H26" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I26" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="27">
@@ -1202,11 +1442,11 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>23000</v>
+        <v>22800</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7633954-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7634532-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1216,12 +1456,21 @@
         <v>3</v>
       </c>
       <c r="F27" t="n">
-        <v>200000</v>
+        <v>298000</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H27" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I27" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="28">
@@ -1231,26 +1480,35 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7633304-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7635502-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E28" t="n">
         <v>3</v>
       </c>
       <c r="F28" t="n">
-        <v>198000</v>
+        <v>260000</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H28" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I28" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="29">
@@ -1260,26 +1518,35 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>20500</v>
+        <v>21000</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7609787-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7627049-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>200000</v>
+        <v>163059</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H29" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I29" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="30">
@@ -1289,26 +1556,35 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>18800</v>
+        <v>22000</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7631416-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7634880-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="E30" t="n">
         <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>234000</v>
+        <v>245368</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H30" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I30" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="31">
@@ -1318,11 +1594,11 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>23500</v>
+        <v>23000</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7583411-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7633954-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1332,12 +1608,21 @@
         <v>3</v>
       </c>
       <c r="F31" t="n">
-        <v>185870</v>
+        <v>200000</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H31" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I31" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="32">
@@ -1347,11 +1632,11 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7628404-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7633304-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1361,12 +1646,21 @@
         <v>3</v>
       </c>
       <c r="F32" t="n">
-        <v>307456</v>
+        <v>198000</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H32" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I32" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="33">
@@ -1376,26 +1670,35 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>23300</v>
+        <v>20500</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7628220-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7609787-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="E33" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>230000</v>
+        <v>200000</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H33" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I33" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="34">
@@ -1405,26 +1708,35 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>22600</v>
+        <v>18800</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7628126-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7631416-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="E34" t="n">
         <v>3</v>
       </c>
       <c r="F34" t="n">
-        <v>269000</v>
+        <v>234000</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H34" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I34" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="35">
@@ -1434,26 +1746,35 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>24600</v>
+        <v>23500</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7627593-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7583411-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D35" t="n">
         <v>2007</v>
       </c>
       <c r="E35" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F35" t="n">
-        <v>347000</v>
+        <v>185870</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H35" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I35" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="36">
@@ -1463,11 +1784,11 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>21750</v>
+        <v>21000</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7627379-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7628404-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1477,12 +1798,21 @@
         <v>3</v>
       </c>
       <c r="F36" t="n">
-        <v>240000</v>
+        <v>307456</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H36" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I36" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J36" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="37">
@@ -1492,26 +1822,35 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>20000</v>
+        <v>23300</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7624790-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7628220-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="E37" t="n">
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="F37" t="n">
-        <v>206000</v>
+        <v>230000</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H37" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I37" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J37" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="38">
@@ -1521,26 +1860,35 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>22500</v>
+        <v>22600</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7571267-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7628126-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E38" t="n">
         <v>3</v>
       </c>
       <c r="F38" t="n">
-        <v>220000</v>
+        <v>269000</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H38" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I38" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J38" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="39">
@@ -1550,26 +1898,35 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>22000</v>
+        <v>24600</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7623871-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7627593-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D39" t="n">
         <v>2007</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F39" t="n">
-        <v>230000</v>
+        <v>347000</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H39" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I39" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="40">
@@ -1579,11 +1936,11 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>23500</v>
+        <v>21750</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7623260-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7627379-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1593,12 +1950,21 @@
         <v>3</v>
       </c>
       <c r="F40" t="n">
-        <v>209000</v>
+        <v>240000</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H40" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I40" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="41">
@@ -1608,11 +1974,11 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>21600</v>
+        <v>22500</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7525562-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7571267-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1622,12 +1988,21 @@
         <v>3</v>
       </c>
       <c r="F41" t="n">
-        <v>209000</v>
+        <v>220000</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H41" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I41" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="42">
@@ -1637,11 +2012,11 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>19800</v>
+        <v>22000</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7620021-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7623871-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1651,12 +2026,21 @@
         <v>3</v>
       </c>
       <c r="F42" t="n">
-        <v>400000</v>
+        <v>230000</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H42" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I42" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J42" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="43">
@@ -1666,26 +2050,35 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>23800</v>
+        <v>22800</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7619309-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7623260-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E43" t="n">
         <v>3</v>
       </c>
       <c r="F43" t="n">
-        <v>201000</v>
+        <v>209000</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H43" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I43" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J43" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="44">
@@ -1695,26 +2088,35 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>18000</v>
+        <v>21600</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7615685-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7525562-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E44" t="n">
         <v>3</v>
       </c>
       <c r="F44" t="n">
-        <v>310000</v>
+        <v>209000</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H44" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I44" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J44" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="45">
@@ -1724,11 +2126,11 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>22500</v>
+        <v>19800</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7566921-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7620021-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1738,12 +2140,21 @@
         <v>3</v>
       </c>
       <c r="F45" t="n">
-        <v>20000</v>
+        <v>400000</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H45" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I45" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J45" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="46">
@@ -1753,26 +2164,35 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>21400</v>
+        <v>23800</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7614876-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7619309-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E46" t="n">
         <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>262000</v>
+        <v>201000</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H46" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I46" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J46" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="47">
@@ -1782,26 +2202,35 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>25000</v>
+        <v>18000</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7610555-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7615685-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E47" t="n">
         <v>3</v>
       </c>
       <c r="F47" t="n">
-        <v>224000</v>
+        <v>310000</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H47" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I47" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J47" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="48">
@@ -1811,11 +2240,11 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>22000</v>
+        <v>22500</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7602055-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7566921-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1825,12 +2254,21 @@
         <v>3</v>
       </c>
       <c r="F48" t="n">
-        <v>213100</v>
+        <v>20000</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H48" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I48" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J48" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="49">
@@ -1840,11 +2278,11 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>23500</v>
+        <v>21400</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7597414-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7614876-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1854,12 +2292,21 @@
         <v>3</v>
       </c>
       <c r="F49" t="n">
-        <v>196512</v>
+        <v>262000</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H49" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I49" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="50">
@@ -1869,11 +2316,11 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>22300</v>
+        <v>25000</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7596583-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7610555-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1883,12 +2330,21 @@
         <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>254000</v>
+        <v>224000</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H50" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I50" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J50" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="51">
@@ -1898,11 +2354,11 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>22500</v>
+        <v>22000</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7594101-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7602055-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1912,12 +2368,21 @@
         <v>3</v>
       </c>
       <c r="F51" t="n">
-        <v>222000</v>
+        <v>213100</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H51" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I51" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J51" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="52">
@@ -1927,11 +2392,11 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>19600</v>
+        <v>23500</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7592780-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7597414-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1941,12 +2406,21 @@
         <v>3</v>
       </c>
       <c r="F52" t="n">
-        <v>315394</v>
+        <v>196512</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H52" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I52" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="53">
@@ -1956,26 +2430,35 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>17200</v>
+        <v>22300</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7586906-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7596583-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E53" t="n">
         <v>3</v>
       </c>
       <c r="F53" t="n">
-        <v>256772</v>
+        <v>254000</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H53" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I53" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="54">
@@ -1985,11 +2468,11 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7582820-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7594101-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1999,12 +2482,21 @@
         <v>3</v>
       </c>
       <c r="F54" t="n">
-        <v>206500</v>
+        <v>222000</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H54" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I54" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J54" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="55">
@@ -2014,26 +2506,35 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>19900</v>
+        <v>19600</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7581565-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7592780-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E55" t="n">
         <v>3</v>
       </c>
       <c r="F55" t="n">
-        <v>321200</v>
+        <v>315394</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H55" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I55" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J55" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="56">
@@ -2043,26 +2544,35 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>22500</v>
+        <v>17200</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7580794-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7586906-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E56" t="n">
         <v>3</v>
       </c>
       <c r="F56" t="n">
-        <v>207333</v>
+        <v>256772</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H56" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I56" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J56" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="57">
@@ -2072,26 +2582,35 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>21200</v>
+        <v>19900</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7579963-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7581565-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="E57" t="n">
         <v>3</v>
       </c>
       <c r="F57" t="n">
-        <v>194000</v>
+        <v>321200</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H57" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I57" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J57" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="58">
@@ -2101,26 +2620,35 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>19000</v>
+        <v>22500</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7579370-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7580794-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E58" t="n">
         <v>3</v>
       </c>
       <c r="F58" t="n">
-        <v>267000</v>
+        <v>207333</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H58" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I58" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J58" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="59">
@@ -2130,11 +2658,11 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>22000</v>
+        <v>21000</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7579273-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7579963-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -2144,12 +2672,21 @@
         <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>229350</v>
+        <v>194000</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H59" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I59" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J59" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="60">
@@ -2159,26 +2696,35 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>24800</v>
+        <v>19000</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7577354-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7579370-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E60" t="n">
         <v>3</v>
       </c>
       <c r="F60" t="n">
-        <v>187000</v>
+        <v>267000</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H60" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I60" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J60" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="61">
@@ -2188,11 +2734,11 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>25000</v>
+        <v>22000</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7575628-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7579273-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -2202,12 +2748,21 @@
         <v>3</v>
       </c>
       <c r="F61" t="n">
-        <v>332767</v>
+        <v>229350</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H61" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I61" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J61" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="62">
@@ -2217,11 +2772,11 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>22500</v>
+        <v>24800</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7560222-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7577354-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -2231,12 +2786,21 @@
         <v>3</v>
       </c>
       <c r="F62" t="n">
-        <v>193000</v>
+        <v>187000</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H62" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I62" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J62" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="63">
@@ -2246,11 +2810,11 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>21800</v>
+        <v>25000</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7571881-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7575628-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2260,12 +2824,21 @@
         <v>3</v>
       </c>
       <c r="F63" t="n">
-        <v>180111</v>
+        <v>332767</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H63" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I63" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J63" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="64">
@@ -2275,26 +2848,35 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>25000</v>
+        <v>21800</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7461672-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7571881-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E64" t="n">
         <v>3</v>
       </c>
       <c r="F64" t="n">
-        <v>430000</v>
+        <v>180111</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
+      </c>
+      <c r="H64" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I64" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J64" t="n">
+        <v>2007</v>
       </c>
     </row>
     <row r="65">
@@ -2304,171 +2886,35 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>17200</v>
+        <v>25000</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://ru.turbo.az/autos/7565192-mitsubishi-pajero</t>
+          <t>https://ru.turbo.az/autos/7461672-mitsubishi-pajero</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="E65" t="n">
         <v>3</v>
       </c>
       <c r="F65" t="n">
-        <v>490000</v>
+        <v>430000</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
           <t>Mitsubishi</t>
         </is>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Mitsubishi Pajero</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>24500</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>https://ru.turbo.az/autos/7560209-mitsubishi-pajero</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>2007</v>
-      </c>
-      <c r="E66" t="n">
-        <v>3</v>
-      </c>
-      <c r="F66" t="n">
-        <v>163094</v>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Mitsubishi</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Mitsubishi Pajero</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>22500</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>https://ru.turbo.az/autos/7562700-mitsubishi-pajero</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>2008</v>
-      </c>
-      <c r="E67" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="F67" t="n">
-        <v>258000</v>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Mitsubishi</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Mitsubishi Pajero</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>21000</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>https://ru.turbo.az/autos/7561295-mitsubishi-pajero</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E68" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="F68" t="n">
-        <v>40000</v>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Mitsubishi</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Mitsubishi Pajero</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>23000</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>https://ru.turbo.az/autos/7468730-mitsubishi-pajero</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>2007</v>
-      </c>
-      <c r="E69" t="n">
-        <v>3</v>
-      </c>
-      <c r="F69" t="n">
-        <v>248000</v>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Mitsubishi</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Mitsubishi Pajero</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>23800</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>https://ru.turbo.az/autos/7558868-mitsubishi-pajero</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>2007</v>
-      </c>
-      <c r="E70" t="n">
-        <v>3</v>
-      </c>
-      <c r="F70" t="n">
-        <v>187000</v>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Mitsubishi</t>
-        </is>
+      <c r="H65" t="n">
+        <v>22500</v>
+      </c>
+      <c r="I65" t="n">
+        <v>224500</v>
+      </c>
+      <c r="J65" t="n">
+        <v>2007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>